<commit_message>
fix: set array to list for number of eventbrite
</commit_message>
<xml_diff>
--- a/skoring/utils/datasets/Result History.xlsx
+++ b/skoring/utils/datasets/Result History.xlsx
@@ -390,17 +390,17 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="25.85546875" customWidth="1" min="1" max="1"/>
+    <col width="24.42578125" customWidth="1" min="1" max="1"/>
     <col width="25.140625" customWidth="1" min="2" max="2"/>
-    <col width="76.7109375" customWidth="1" min="3" max="3"/>
+    <col width="61.140625" customWidth="1" min="3" max="3"/>
     <col width="20.42578125" customWidth="1" min="4" max="4"/>
     <col width="53.7109375" customWidth="1" min="5" max="5"/>
     <col width="21.28515625" customWidth="1" min="6" max="6"/>
@@ -602,8 +602,6 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr"/>
-      <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
           <t>Microsoft Security, Compliance, and Identity Fundamentals</t>
@@ -614,8 +612,6 @@
           <t>0.41301278095468785</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr">
         <is>
           <t>microsoft 365</t>
@@ -634,12 +630,6 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr"/>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr">
         <is>
           <t>office</t>
@@ -656,6 +646,646 @@
       <c r="J7" t="n">
         <v>2286802</v>
       </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>pelatihan microsoft 365</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>azure,microsoft 365,office</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>BPK Penabur Series: PowerShell Administration</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>0.3474523756848368</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Microsoft 365 Fundamentals</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>1.9740553522229207</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>azure</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>43</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>azure</t>
+        </is>
+      </c>
+      <c r="J8" t="n">
+        <v>58984</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Building The Integrated Virtual Classroom with Teams and Moodle</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>0.3748262036910711</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Office 365 Administrator</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>0.22034156494338966</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>microsoft 365</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>7</v>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>microsoft 365</t>
+        </is>
+      </c>
+      <c r="J9" t="n">
+        <v>33577</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Building Virtual Classroom with Teams</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>0.6365736740597923</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>office</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>12</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>office</t>
+        </is>
+      </c>
+      <c r="J10" t="n">
+        <v>2284093</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Creating An App Solution for Higher Ed Institution with Power Platforms</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>0.7082311065875776</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Creating and Managing a Document Academic using Office 365</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>1.3590070992011116</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Enabling Microsoft 365 Workloads for Collaboration</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>0.26272055141994044</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>FunFest - Microsoft 365—Get to know Microsoft 365 as a University Facility</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>0.6034080308500449</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr"/>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Global Microsoft 365 Developer Bootcamp 2019</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>0.26776639227643884</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr"/>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Global Microsoft 365 Developer Bootcamp 2020</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>0.2564933145830506</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr"/>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>How to Create a Multimedia Learning Object with Various Tools</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>0.3748262036910711</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr"/>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Inclusive Learning with Microsoft 365 </t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>0.23651354312606715</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr"/>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Introduction to Microsoft 365</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>0.5851324366935264</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr"/>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Managing Lecture Notes Digitally with OneNote</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>0.3371999958246887</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr"/>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Microsoft 365 Admin Center and Azure DevOps</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>0.49756394776087876</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr"/>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Microsoft 365 Administration Workshop</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>1.7183431043388944</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr"/>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Microsoft 365 Enterprise and Security Administration and EFO App</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>0.9929760104202436</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr"/>
+      <c r="J23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr"/>
+      <c r="B24" t="inlineStr"/>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Microsoft 365 Identity with Azure Active Directory</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>0.21541730269874618</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr"/>
+      <c r="J24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr"/>
+      <c r="B25" t="inlineStr"/>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Microsoft 365 Identity with Azure Active Directory </t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>0.21541730269874618</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="inlineStr"/>
+      <c r="J25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr"/>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Microsoft 365 Overview</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>0.5103790337486951</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr"/>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Microsoft 365 for Improving Productivity</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>0.6365736740597923</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr"/>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Office 365 Learning Utilization Training (Microsoft 365 Account Activation and Microsoft Educator Center Exploration)</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>0.28014128030482593</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr"/>
+      <c r="B29" t="inlineStr"/>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Optimizing Microsoft 365 for College Student</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>0.35273685300602203</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="inlineStr"/>
+      <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="inlineStr"/>
+      <c r="J29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr"/>
+      <c r="B30" t="inlineStr"/>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PowerShell Workshop </t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>0.207606437583086</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr"/>
+      <c r="F30" t="inlineStr"/>
+      <c r="G30" t="inlineStr"/>
+      <c r="H30" t="inlineStr"/>
+      <c r="I30" t="inlineStr"/>
+      <c r="J30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr"/>
+      <c r="B31" t="inlineStr"/>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Project Collaboration using Teams and Planner</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>0.3748262036910711</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="inlineStr"/>
+      <c r="G31" t="inlineStr"/>
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="inlineStr"/>
+      <c r="J31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr"/>
+      <c r="B32" t="inlineStr"/>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Research and Reference Data Management</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>0.330125069941719</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="inlineStr"/>
+      <c r="G32" t="inlineStr"/>
+      <c r="H32" t="inlineStr"/>
+      <c r="I32" t="inlineStr"/>
+      <c r="J32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr"/>
+      <c r="B33" t="inlineStr"/>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Save Classroom Time tools for planning, assignments</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>0.5890962384372053</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="inlineStr"/>
+      <c r="G33" t="inlineStr"/>
+      <c r="H33" t="inlineStr"/>
+      <c r="I33" t="inlineStr"/>
+      <c r="J33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr"/>
+      <c r="B34" t="inlineStr"/>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Teacher Skill Improvement</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>0.3382433248462924</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr"/>
+      <c r="F34" t="inlineStr"/>
+      <c r="G34" t="inlineStr"/>
+      <c r="H34" t="inlineStr"/>
+      <c r="I34" t="inlineStr"/>
+      <c r="J34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr"/>
+      <c r="B35" t="inlineStr"/>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Tracking The Successful of Learning in Higher Ed with Power BI</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>0.3541155532937888</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr"/>
+      <c r="F35" t="inlineStr"/>
+      <c r="G35" t="inlineStr"/>
+      <c r="H35" t="inlineStr"/>
+      <c r="I35" t="inlineStr"/>
+      <c r="J35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr"/>
+      <c r="B36" t="inlineStr"/>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Workshop Microsoft 365 - Word for Academic Research</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>0.35273685300602203</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr"/>
+      <c r="F36" t="inlineStr"/>
+      <c r="G36" t="inlineStr"/>
+      <c r="H36" t="inlineStr"/>
+      <c r="I36" t="inlineStr"/>
+      <c r="J36" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix: max average values
</commit_message>
<xml_diff>
--- a/skoring/utils/datasets/Result History.xlsx
+++ b/skoring/utils/datasets/Result History.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
@@ -696,8 +696,6 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr"/>
-      <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr">
         <is>
           <t>Building The Integrated Virtual Classroom with Teams and Moodle</t>
@@ -736,8 +734,6 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr"/>
-      <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr">
         <is>
           <t>Building Virtual Classroom with Teams</t>
@@ -748,8 +744,6 @@
           <t>0.6365736740597923</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr">
         <is>
           <t>office</t>
@@ -768,8 +762,6 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr"/>
-      <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr">
         <is>
           <t>Creating An App Solution for Higher Ed Institution with Power Platforms</t>
@@ -780,16 +772,8 @@
           <t>0.7082311065875776</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr"/>
-      <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr">
         <is>
           <t>Creating and Managing a Document Academic using Office 365</t>
@@ -800,16 +784,8 @@
           <t>1.3590070992011116</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr"/>
-      <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr">
         <is>
           <t>Enabling Microsoft 365 Workloads for Collaboration</t>
@@ -820,16 +796,8 @@
           <t>0.26272055141994044</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr"/>
-      <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr">
         <is>
           <t>FunFest - Microsoft 365—Get to know Microsoft 365 as a University Facility</t>
@@ -840,16 +808,8 @@
           <t>0.6034080308500449</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr"/>
-      <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr">
         <is>
           <t>Global Microsoft 365 Developer Bootcamp 2019</t>
@@ -860,16 +820,8 @@
           <t>0.26776639227643884</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr"/>
-      <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr">
         <is>
           <t>Global Microsoft 365 Developer Bootcamp 2020</t>
@@ -880,16 +832,8 @@
           <t>0.2564933145830506</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr"/>
-      <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr">
         <is>
           <t>How to Create a Multimedia Learning Object with Various Tools</t>
@@ -900,16 +844,8 @@
           <t>0.3748262036910711</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr"/>
-      <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr">
         <is>
           <t xml:space="preserve">Inclusive Learning with Microsoft 365 </t>
@@ -920,16 +856,8 @@
           <t>0.23651354312606715</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
-      <c r="J18" t="inlineStr"/>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr"/>
-      <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr">
         <is>
           <t>Introduction to Microsoft 365</t>
@@ -940,16 +868,8 @@
           <t>0.5851324366935264</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
-      <c r="J19" t="inlineStr"/>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr"/>
-      <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr">
         <is>
           <t>Managing Lecture Notes Digitally with OneNote</t>
@@ -960,16 +880,8 @@
           <t>0.3371999958246887</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr"/>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr"/>
-      <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr">
         <is>
           <t>Microsoft 365 Admin Center and Azure DevOps</t>
@@ -980,16 +892,8 @@
           <t>0.49756394776087876</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr"/>
-      <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr">
         <is>
           <t>Microsoft 365 Administration Workshop</t>
@@ -1000,16 +904,8 @@
           <t>1.7183431043388944</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr"/>
-      <c r="J22" t="inlineStr"/>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr"/>
-      <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr">
         <is>
           <t>Microsoft 365 Enterprise and Security Administration and EFO App</t>
@@ -1020,16 +916,8 @@
           <t>0.9929760104202436</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
-      <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr"/>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr"/>
-      <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr">
         <is>
           <t>Microsoft 365 Identity with Azure Active Directory</t>
@@ -1040,16 +928,8 @@
           <t>0.21541730269874618</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr"/>
-      <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr"/>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr"/>
-      <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr">
         <is>
           <t xml:space="preserve">Microsoft 365 Identity with Azure Active Directory </t>
@@ -1060,16 +940,8 @@
           <t>0.21541730269874618</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr"/>
-      <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr"/>
-      <c r="H25" t="inlineStr"/>
-      <c r="I25" t="inlineStr"/>
-      <c r="J25" t="inlineStr"/>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr"/>
-      <c r="B26" t="inlineStr"/>
       <c r="C26" t="inlineStr">
         <is>
           <t>Microsoft 365 Overview</t>
@@ -1080,16 +952,8 @@
           <t>0.5103790337486951</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr"/>
-      <c r="I26" t="inlineStr"/>
-      <c r="J26" t="inlineStr"/>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr"/>
-      <c r="B27" t="inlineStr"/>
       <c r="C27" t="inlineStr">
         <is>
           <t>Microsoft 365 for Improving Productivity</t>
@@ -1100,16 +964,8 @@
           <t>0.6365736740597923</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr"/>
-      <c r="F27" t="inlineStr"/>
-      <c r="G27" t="inlineStr"/>
-      <c r="H27" t="inlineStr"/>
-      <c r="I27" t="inlineStr"/>
-      <c r="J27" t="inlineStr"/>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr"/>
-      <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr">
         <is>
           <t>Office 365 Learning Utilization Training (Microsoft 365 Account Activation and Microsoft Educator Center Exploration)</t>
@@ -1120,16 +976,8 @@
           <t>0.28014128030482593</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr"/>
-      <c r="F28" t="inlineStr"/>
-      <c r="G28" t="inlineStr"/>
-      <c r="H28" t="inlineStr"/>
-      <c r="I28" t="inlineStr"/>
-      <c r="J28" t="inlineStr"/>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr"/>
-      <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr">
         <is>
           <t>Optimizing Microsoft 365 for College Student</t>
@@ -1140,16 +988,8 @@
           <t>0.35273685300602203</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr"/>
-      <c r="F29" t="inlineStr"/>
-      <c r="G29" t="inlineStr"/>
-      <c r="H29" t="inlineStr"/>
-      <c r="I29" t="inlineStr"/>
-      <c r="J29" t="inlineStr"/>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr"/>
-      <c r="B30" t="inlineStr"/>
       <c r="C30" t="inlineStr">
         <is>
           <t xml:space="preserve">PowerShell Workshop </t>
@@ -1160,16 +1000,8 @@
           <t>0.207606437583086</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr"/>
-      <c r="F30" t="inlineStr"/>
-      <c r="G30" t="inlineStr"/>
-      <c r="H30" t="inlineStr"/>
-      <c r="I30" t="inlineStr"/>
-      <c r="J30" t="inlineStr"/>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr"/>
-      <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr">
         <is>
           <t>Project Collaboration using Teams and Planner</t>
@@ -1180,16 +1012,8 @@
           <t>0.3748262036910711</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr"/>
-      <c r="F31" t="inlineStr"/>
-      <c r="G31" t="inlineStr"/>
-      <c r="H31" t="inlineStr"/>
-      <c r="I31" t="inlineStr"/>
-      <c r="J31" t="inlineStr"/>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr"/>
-      <c r="B32" t="inlineStr"/>
       <c r="C32" t="inlineStr">
         <is>
           <t>Research and Reference Data Management</t>
@@ -1200,16 +1024,8 @@
           <t>0.330125069941719</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr"/>
-      <c r="F32" t="inlineStr"/>
-      <c r="G32" t="inlineStr"/>
-      <c r="H32" t="inlineStr"/>
-      <c r="I32" t="inlineStr"/>
-      <c r="J32" t="inlineStr"/>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr"/>
-      <c r="B33" t="inlineStr"/>
       <c r="C33" t="inlineStr">
         <is>
           <t>Save Classroom Time tools for planning, assignments</t>
@@ -1220,16 +1036,8 @@
           <t>0.5890962384372053</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr"/>
-      <c r="F33" t="inlineStr"/>
-      <c r="G33" t="inlineStr"/>
-      <c r="H33" t="inlineStr"/>
-      <c r="I33" t="inlineStr"/>
-      <c r="J33" t="inlineStr"/>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr"/>
-      <c r="B34" t="inlineStr"/>
       <c r="C34" t="inlineStr">
         <is>
           <t>Teacher Skill Improvement</t>
@@ -1240,16 +1048,8 @@
           <t>0.3382433248462924</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr"/>
-      <c r="F34" t="inlineStr"/>
-      <c r="G34" t="inlineStr"/>
-      <c r="H34" t="inlineStr"/>
-      <c r="I34" t="inlineStr"/>
-      <c r="J34" t="inlineStr"/>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr"/>
-      <c r="B35" t="inlineStr"/>
       <c r="C35" t="inlineStr">
         <is>
           <t>Tracking The Successful of Learning in Higher Ed with Power BI</t>
@@ -1260,16 +1060,8 @@
           <t>0.3541155532937888</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr"/>
-      <c r="F35" t="inlineStr"/>
-      <c r="G35" t="inlineStr"/>
-      <c r="H35" t="inlineStr"/>
-      <c r="I35" t="inlineStr"/>
-      <c r="J35" t="inlineStr"/>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr"/>
-      <c r="B36" t="inlineStr"/>
       <c r="C36" t="inlineStr">
         <is>
           <t>Workshop Microsoft 365 - Word for Academic Research</t>
@@ -1280,12 +1072,598 @@
           <t>0.35273685300602203</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr"/>
-      <c r="F36" t="inlineStr"/>
-      <c r="G36" t="inlineStr"/>
-      <c r="H36" t="inlineStr"/>
-      <c r="I36" t="inlineStr"/>
-      <c r="J36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>power BI</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>data analyst,business analyst</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Advanced Power BI</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>0.608004566787522</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Analyzing Data with Power BI</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>2.633071549589857</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>data analyst</t>
+        </is>
+      </c>
+      <c r="H37" t="n">
+        <v>98</v>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>data analyst</t>
+        </is>
+      </c>
+      <c r="J37" t="n">
+        <v>14027</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Data Visualization with Microsoft Power BI</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>0.8691866597611404</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Analyzing Data with Power BI - Series 1</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>2.660842091301512</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>business analyst</t>
+        </is>
+      </c>
+      <c r="H38" t="n">
+        <v>147</v>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>business analyst</t>
+        </is>
+      </c>
+      <c r="J38" t="n">
+        <v>2347</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Microsoft Power Platform Fundamentals</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>0.5487337283521597</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Analyzing Data with Power BI - Series 2</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>2.414102362428948</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Power BI Advanced</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>2.3019120804914768</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Microsoft Power Platform App Maker</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>0.7955862426861524</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Power BI Essentials</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>1.5452437265224108</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Microsoft Power Platform Functional Consultant</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>0.5173586175710994</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Tracking The Successful of Learning in Higher Ed with Power BI</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>0.8293929887336926</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Microsoft Power Platform Fundamentals</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>0.6617981329674373</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Visualize Student Performance Data Using Power BI</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>0.44404010896584</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>power BI</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>data analyst,business analyst</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Advanced Power BI</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>0.608004566787522</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Analyzing Data with Power BI</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>2.633071549589857</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>data analyst</t>
+        </is>
+      </c>
+      <c r="H44" t="n">
+        <v>98</v>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>data analyst</t>
+        </is>
+      </c>
+      <c r="J44" t="n">
+        <v>14030</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Data Visualization with Microsoft Power BI</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>0.8691866597611404</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Analyzing Data with Power BI - Series 1</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>2.660842091301512</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>business analyst</t>
+        </is>
+      </c>
+      <c r="H45" t="n">
+        <v>147</v>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>business analyst</t>
+        </is>
+      </c>
+      <c r="J45" t="n">
+        <v>2349</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Microsoft Power Platform Fundamentals</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>0.5487337283521597</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Analyzing Data with Power BI - Series 2</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>2.414102362428948</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Power BI Advanced</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>2.3019120804914768</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Microsoft Power Platform App Maker</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>0.7955862426861524</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Power BI Essentials</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>1.5452437265224108</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Microsoft Power Platform Functional Consultant</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>0.5173586175710994</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Tracking The Successful of Learning in Higher Ed with Power BI</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>0.8293929887336926</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Microsoft Power Platform Fundamentals</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>0.6617981329674373</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Visualize Student Performance Data Using Power BI</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>0.44404010896584</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>power BI</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>data analyst,business analyst</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Advanced Power BI</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>0.608004566787522</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Analyzing Data with Power BI</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>2.633071549589857</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>data analyst</t>
+        </is>
+      </c>
+      <c r="H51" t="n">
+        <v>98</v>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>data analyst</t>
+        </is>
+      </c>
+      <c r="J51" t="n">
+        <v>14029</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr"/>
+      <c r="B52" t="inlineStr"/>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Data Visualization with Microsoft Power BI</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>0.8691866597611404</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Analyzing Data with Power BI - Series 1</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>2.660842091301512</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>business analyst</t>
+        </is>
+      </c>
+      <c r="H52" t="n">
+        <v>147</v>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>business analyst</t>
+        </is>
+      </c>
+      <c r="J52" t="n">
+        <v>2349</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr"/>
+      <c r="B53" t="inlineStr"/>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Microsoft Power Platform Fundamentals</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>0.5487337283521597</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Analyzing Data with Power BI - Series 2</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>2.414102362428948</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr"/>
+      <c r="H53" t="inlineStr"/>
+      <c r="I53" t="inlineStr"/>
+      <c r="J53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr"/>
+      <c r="B54" t="inlineStr"/>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Power BI Advanced</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>2.3019120804914768</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Microsoft Power Platform App Maker</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>0.7955862426861524</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr"/>
+      <c r="H54" t="inlineStr"/>
+      <c r="I54" t="inlineStr"/>
+      <c r="J54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr"/>
+      <c r="B55" t="inlineStr"/>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Power BI Essentials</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>1.5452437265224108</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Microsoft Power Platform Functional Consultant</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>0.5173586175710994</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr"/>
+      <c r="H55" t="inlineStr"/>
+      <c r="I55" t="inlineStr"/>
+      <c r="J55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr"/>
+      <c r="B56" t="inlineStr"/>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Tracking The Successful of Learning in Higher Ed with Power BI</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>0.8293929887336926</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Microsoft Power Platform Fundamentals</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>0.6617981329674373</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr"/>
+      <c r="H56" t="inlineStr"/>
+      <c r="I56" t="inlineStr"/>
+      <c r="J56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr"/>
+      <c r="B57" t="inlineStr"/>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Visualize Student Performance Data Using Power BI</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>0.44404010896584</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr"/>
+      <c r="F57" t="inlineStr"/>
+      <c r="G57" t="inlineStr"/>
+      <c r="H57" t="inlineStr"/>
+      <c r="I57" t="inlineStr"/>
+      <c r="J57" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: replace twitter to pytrend
</commit_message>
<xml_diff>
--- a/skoring/utils/datasets/Result History.xlsx
+++ b/skoring/utils/datasets/Result History.xlsx
@@ -1,79 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repository\sistem-skoring-pelatihan-microsoft\skoring\utils\datasets\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68CFF843-EC39-49EF-89AE-DE5D1CD828D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>Query</t>
-  </si>
-  <si>
-    <t>Topics</t>
-  </si>
-  <si>
-    <t>Hasil Event</t>
-  </si>
-  <si>
-    <t>Skor Event</t>
-  </si>
-  <si>
-    <t>Hasil Katalog</t>
-  </si>
-  <si>
-    <t>Skor Katalog</t>
-  </si>
-  <si>
-    <t>Hasil Eventbrite</t>
-  </si>
-  <si>
-    <t>Skor Eventbrite</t>
-  </si>
-  <si>
-    <t>Topik Twitter</t>
-  </si>
-  <si>
-    <t>Start Date</t>
-  </si>
-  <si>
-    <t>End Date</t>
-  </si>
-  <si>
-    <t>Tweet Count</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -92,21 +46,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -372,63 +385,234 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" customWidth="1"/>
-    <col min="3" max="3" width="35.28515625" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" customWidth="1"/>
-    <col min="5" max="5" width="26.85546875" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" customWidth="1"/>
-    <col min="7" max="9" width="16.7109375" customWidth="1"/>
-    <col min="10" max="10" width="25" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.42578125" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" customWidth="1"/>
+    <col width="24.42578125" customWidth="1" min="1" max="1"/>
+    <col width="25.140625" customWidth="1" min="2" max="2"/>
+    <col width="35.28515625" customWidth="1" min="3" max="3"/>
+    <col width="20.42578125" customWidth="1" min="4" max="4"/>
+    <col width="26.85546875" customWidth="1" min="5" max="5"/>
+    <col width="21.28515625" customWidth="1" min="6" max="6"/>
+    <col width="23.42578125" customWidth="1" min="7" max="7"/>
+    <col width="16.7109375" customWidth="1" min="8" max="9"/>
+    <col width="25" bestFit="1" customWidth="1" min="10" max="10"/>
+    <col width="25.42578125" customWidth="1" min="11" max="11"/>
+    <col width="11.42578125" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Query</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Topics</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Hasil Event</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Skor Event</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Hasil Katalog</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Skor Katalog</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Hasil Eventbrite</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Skor Eventbrite</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Topik Google Trend</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Hasil Google Trend</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>pelatihan microsoft azure</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>google drive,google cloud platform,microsoft azure,chatgpt,gpt-4</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>6 Steps to Get Started Deploying Cloud Computing in Schools with Azure for Education</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>0.3121013001740982</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Microsoft Security, Compliance, and Identity Fundamentals</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>0.47722590822176536</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>google drive</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>33</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>google drive</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr"/>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Microsoft Security, Compliance, and Identity Fundamentals</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>0.4134549694332694</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>google cloud platform</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>13</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>google cloud platform</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>microsoft azure</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>6</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>microsoft azure</t>
+        </is>
+      </c>
+      <c r="J4" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>chatgpt</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>chatgpt</t>
+        </is>
+      </c>
+      <c r="J5" t="n">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>gpt-4</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>99</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>gpt-4</t>
+        </is>
+      </c>
+      <c r="J6" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>